<commit_message>
Adds a draft mechanism to calculate the present value of future industrial carbon prices, giving producers insight into future investment costs (#355)
</commit_message>
<xml_diff>
--- a/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
+++ b/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\fuels\BCTR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\fuels\BCTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ED464C-FC0C-47EF-A2C1-21B0B5CF6166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFB306A-97BD-4018-B5E8-3691A0AC6A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="435" windowWidth="23955" windowHeight="16500" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
+    <workbookView xWindow="5970" yWindow="2430" windowWidth="21600" windowHeight="12525" activeTab="1" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -199,7 +199,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -305,7 +305,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -447,7 +447,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -457,16 +457,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49357908-BC85-41CC-9D98-173369A13AF6}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -474,17 +474,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -500,117 +500,264 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:CC9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
+    <col min="31" max="31" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1" s="1">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="D1" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="E1" s="1">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="F1" s="1">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="G1" s="1">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="H1" s="1">
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="I1" s="1">
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="J1" s="1">
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="K1" s="1">
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="L1" s="1">
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="M1" s="1">
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="N1" s="1">
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="O1" s="1">
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="P1" s="1">
-        <v>2033</v>
+        <v>2035</v>
       </c>
       <c r="Q1" s="1">
-        <v>2034</v>
+        <v>2036</v>
       </c>
       <c r="R1" s="1">
-        <v>2035</v>
+        <v>2037</v>
       </c>
       <c r="S1" s="1">
-        <v>2036</v>
+        <v>2038</v>
       </c>
       <c r="T1" s="1">
-        <v>2037</v>
+        <v>2039</v>
       </c>
       <c r="U1" s="1">
-        <v>2038</v>
+        <v>2040</v>
       </c>
       <c r="V1" s="1">
-        <v>2039</v>
+        <v>2041</v>
       </c>
       <c r="W1" s="1">
-        <v>2040</v>
+        <v>2042</v>
       </c>
       <c r="X1" s="1">
-        <v>2041</v>
+        <v>2043</v>
       </c>
       <c r="Y1" s="1">
-        <v>2042</v>
+        <v>2044</v>
       </c>
       <c r="Z1" s="1">
-        <v>2043</v>
+        <v>2045</v>
       </c>
       <c r="AA1" s="1">
-        <v>2044</v>
+        <v>2046</v>
       </c>
       <c r="AB1" s="1">
-        <v>2045</v>
+        <v>2047</v>
       </c>
       <c r="AC1" s="1">
-        <v>2046</v>
+        <v>2048</v>
       </c>
       <c r="AD1" s="1">
-        <v>2047</v>
+        <v>2049</v>
       </c>
       <c r="AE1" s="1">
-        <v>2048</v>
+        <v>2050</v>
       </c>
       <c r="AF1" s="1">
-        <v>2049</v>
+        <v>2051</v>
       </c>
       <c r="AG1" s="1">
-        <v>2050</v>
+        <v>2052</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>2053</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>2054</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>2055</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>2056</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>2057</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>2058</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>2059</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>2060</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>2061</v>
+      </c>
+      <c r="AQ1" s="1">
+        <v>2062</v>
+      </c>
+      <c r="AR1" s="1">
+        <v>2063</v>
+      </c>
+      <c r="AS1" s="1">
+        <v>2064</v>
+      </c>
+      <c r="AT1" s="1">
+        <v>2065</v>
+      </c>
+      <c r="AU1" s="1">
+        <v>2066</v>
+      </c>
+      <c r="AV1" s="1">
+        <v>2067</v>
+      </c>
+      <c r="AW1" s="1">
+        <v>2068</v>
+      </c>
+      <c r="AX1" s="1">
+        <v>2069</v>
+      </c>
+      <c r="AY1" s="1">
+        <v>2070</v>
+      </c>
+      <c r="AZ1" s="1">
+        <v>2071</v>
+      </c>
+      <c r="BA1" s="1">
+        <v>2072</v>
+      </c>
+      <c r="BB1" s="1">
+        <v>2073</v>
+      </c>
+      <c r="BC1" s="1">
+        <v>2074</v>
+      </c>
+      <c r="BD1" s="1">
+        <v>2075</v>
+      </c>
+      <c r="BE1" s="1">
+        <v>2076</v>
+      </c>
+      <c r="BF1" s="1">
+        <v>2077</v>
+      </c>
+      <c r="BG1" s="1">
+        <v>2078</v>
+      </c>
+      <c r="BH1" s="1">
+        <v>2079</v>
+      </c>
+      <c r="BI1" s="1">
+        <v>2080</v>
+      </c>
+      <c r="BJ1" s="1">
+        <v>2081</v>
+      </c>
+      <c r="BK1" s="1">
+        <v>2082</v>
+      </c>
+      <c r="BL1" s="1">
+        <v>2083</v>
+      </c>
+      <c r="BM1" s="1">
+        <v>2084</v>
+      </c>
+      <c r="BN1" s="1">
+        <v>2085</v>
+      </c>
+      <c r="BO1" s="1">
+        <v>2086</v>
+      </c>
+      <c r="BP1" s="1">
+        <v>2087</v>
+      </c>
+      <c r="BQ1" s="1">
+        <v>2088</v>
+      </c>
+      <c r="BR1" s="1">
+        <v>2089</v>
+      </c>
+      <c r="BS1" s="1">
+        <v>2090</v>
+      </c>
+      <c r="BT1" s="1">
+        <v>2091</v>
+      </c>
+      <c r="BU1" s="1">
+        <v>2092</v>
+      </c>
+      <c r="BV1" s="1">
+        <v>2093</v>
+      </c>
+      <c r="BW1" s="1">
+        <v>2094</v>
+      </c>
+      <c r="BX1" s="1">
+        <v>2095</v>
+      </c>
+      <c r="BY1" s="1">
+        <v>2096</v>
+      </c>
+      <c r="BZ1" s="1">
+        <v>2097</v>
+      </c>
+      <c r="CA1" s="1">
+        <v>2098</v>
+      </c>
+      <c r="CB1" s="1">
+        <v>2099</v>
+      </c>
+      <c r="CC1" s="1">
+        <v>2100</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -710,8 +857,152 @@
       <c r="AG2">
         <v>0</v>
       </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BF2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+      <c r="BH2">
+        <v>0</v>
+      </c>
+      <c r="BI2">
+        <v>0</v>
+      </c>
+      <c r="BJ2">
+        <v>0</v>
+      </c>
+      <c r="BK2">
+        <v>0</v>
+      </c>
+      <c r="BL2">
+        <v>0</v>
+      </c>
+      <c r="BM2">
+        <v>0</v>
+      </c>
+      <c r="BN2">
+        <v>0</v>
+      </c>
+      <c r="BO2">
+        <v>0</v>
+      </c>
+      <c r="BP2">
+        <v>0</v>
+      </c>
+      <c r="BQ2">
+        <v>0</v>
+      </c>
+      <c r="BR2">
+        <v>0</v>
+      </c>
+      <c r="BS2">
+        <v>0</v>
+      </c>
+      <c r="BT2">
+        <v>0</v>
+      </c>
+      <c r="BU2">
+        <v>0</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
+      <c r="BW2">
+        <v>0</v>
+      </c>
+      <c r="BX2">
+        <v>0</v>
+      </c>
+      <c r="BY2">
+        <v>0</v>
+      </c>
+      <c r="BZ2">
+        <v>0</v>
+      </c>
+      <c r="CA2">
+        <v>0</v>
+      </c>
+      <c r="CB2">
+        <v>0</v>
+      </c>
+      <c r="CC2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -811,8 +1102,152 @@
       <c r="AG3">
         <v>0</v>
       </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="AZ3">
+        <v>0</v>
+      </c>
+      <c r="BA3">
+        <v>0</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3">
+        <v>0</v>
+      </c>
+      <c r="BD3">
+        <v>0</v>
+      </c>
+      <c r="BE3">
+        <v>0</v>
+      </c>
+      <c r="BF3">
+        <v>0</v>
+      </c>
+      <c r="BG3">
+        <v>0</v>
+      </c>
+      <c r="BH3">
+        <v>0</v>
+      </c>
+      <c r="BI3">
+        <v>0</v>
+      </c>
+      <c r="BJ3">
+        <v>0</v>
+      </c>
+      <c r="BK3">
+        <v>0</v>
+      </c>
+      <c r="BL3">
+        <v>0</v>
+      </c>
+      <c r="BM3">
+        <v>0</v>
+      </c>
+      <c r="BN3">
+        <v>0</v>
+      </c>
+      <c r="BO3">
+        <v>0</v>
+      </c>
+      <c r="BP3">
+        <v>0</v>
+      </c>
+      <c r="BQ3">
+        <v>0</v>
+      </c>
+      <c r="BR3">
+        <v>0</v>
+      </c>
+      <c r="BS3">
+        <v>0</v>
+      </c>
+      <c r="BT3">
+        <v>0</v>
+      </c>
+      <c r="BU3">
+        <v>0</v>
+      </c>
+      <c r="BV3">
+        <v>0</v>
+      </c>
+      <c r="BW3">
+        <v>0</v>
+      </c>
+      <c r="BX3">
+        <v>0</v>
+      </c>
+      <c r="BY3">
+        <v>0</v>
+      </c>
+      <c r="BZ3">
+        <v>0</v>
+      </c>
+      <c r="CA3">
+        <v>0</v>
+      </c>
+      <c r="CB3">
+        <v>0</v>
+      </c>
+      <c r="CC3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -912,8 +1347,152 @@
       <c r="AG4">
         <v>0</v>
       </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4">
+        <v>0</v>
+      </c>
+      <c r="BA4">
+        <v>0</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
+      </c>
+      <c r="BD4">
+        <v>0</v>
+      </c>
+      <c r="BE4">
+        <v>0</v>
+      </c>
+      <c r="BF4">
+        <v>0</v>
+      </c>
+      <c r="BG4">
+        <v>0</v>
+      </c>
+      <c r="BH4">
+        <v>0</v>
+      </c>
+      <c r="BI4">
+        <v>0</v>
+      </c>
+      <c r="BJ4">
+        <v>0</v>
+      </c>
+      <c r="BK4">
+        <v>0</v>
+      </c>
+      <c r="BL4">
+        <v>0</v>
+      </c>
+      <c r="BM4">
+        <v>0</v>
+      </c>
+      <c r="BN4">
+        <v>0</v>
+      </c>
+      <c r="BO4">
+        <v>0</v>
+      </c>
+      <c r="BP4">
+        <v>0</v>
+      </c>
+      <c r="BQ4">
+        <v>0</v>
+      </c>
+      <c r="BR4">
+        <v>0</v>
+      </c>
+      <c r="BS4">
+        <v>0</v>
+      </c>
+      <c r="BT4">
+        <v>0</v>
+      </c>
+      <c r="BU4">
+        <v>0</v>
+      </c>
+      <c r="BV4">
+        <v>0</v>
+      </c>
+      <c r="BW4">
+        <v>0</v>
+      </c>
+      <c r="BX4">
+        <v>0</v>
+      </c>
+      <c r="BY4">
+        <v>0</v>
+      </c>
+      <c r="BZ4">
+        <v>0</v>
+      </c>
+      <c r="CA4">
+        <v>0</v>
+      </c>
+      <c r="CB4">
+        <v>0</v>
+      </c>
+      <c r="CC4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1013,8 +1592,152 @@
       <c r="AG5">
         <v>0</v>
       </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="AZ5">
+        <v>0</v>
+      </c>
+      <c r="BA5">
+        <v>0</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+      <c r="BC5">
+        <v>0</v>
+      </c>
+      <c r="BD5">
+        <v>0</v>
+      </c>
+      <c r="BE5">
+        <v>0</v>
+      </c>
+      <c r="BF5">
+        <v>0</v>
+      </c>
+      <c r="BG5">
+        <v>0</v>
+      </c>
+      <c r="BH5">
+        <v>0</v>
+      </c>
+      <c r="BI5">
+        <v>0</v>
+      </c>
+      <c r="BJ5">
+        <v>0</v>
+      </c>
+      <c r="BK5">
+        <v>0</v>
+      </c>
+      <c r="BL5">
+        <v>0</v>
+      </c>
+      <c r="BM5">
+        <v>0</v>
+      </c>
+      <c r="BN5">
+        <v>0</v>
+      </c>
+      <c r="BO5">
+        <v>0</v>
+      </c>
+      <c r="BP5">
+        <v>0</v>
+      </c>
+      <c r="BQ5">
+        <v>0</v>
+      </c>
+      <c r="BR5">
+        <v>0</v>
+      </c>
+      <c r="BS5">
+        <v>0</v>
+      </c>
+      <c r="BT5">
+        <v>0</v>
+      </c>
+      <c r="BU5">
+        <v>0</v>
+      </c>
+      <c r="BV5">
+        <v>0</v>
+      </c>
+      <c r="BW5">
+        <v>0</v>
+      </c>
+      <c r="BX5">
+        <v>0</v>
+      </c>
+      <c r="BY5">
+        <v>0</v>
+      </c>
+      <c r="BZ5">
+        <v>0</v>
+      </c>
+      <c r="CA5">
+        <v>0</v>
+      </c>
+      <c r="CB5">
+        <v>0</v>
+      </c>
+      <c r="CC5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1114,8 +1837,152 @@
       <c r="AG6">
         <v>0</v>
       </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>0</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
+      <c r="AZ6">
+        <v>0</v>
+      </c>
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
+      <c r="BC6">
+        <v>0</v>
+      </c>
+      <c r="BD6">
+        <v>0</v>
+      </c>
+      <c r="BE6">
+        <v>0</v>
+      </c>
+      <c r="BF6">
+        <v>0</v>
+      </c>
+      <c r="BG6">
+        <v>0</v>
+      </c>
+      <c r="BH6">
+        <v>0</v>
+      </c>
+      <c r="BI6">
+        <v>0</v>
+      </c>
+      <c r="BJ6">
+        <v>0</v>
+      </c>
+      <c r="BK6">
+        <v>0</v>
+      </c>
+      <c r="BL6">
+        <v>0</v>
+      </c>
+      <c r="BM6">
+        <v>0</v>
+      </c>
+      <c r="BN6">
+        <v>0</v>
+      </c>
+      <c r="BO6">
+        <v>0</v>
+      </c>
+      <c r="BP6">
+        <v>0</v>
+      </c>
+      <c r="BQ6">
+        <v>0</v>
+      </c>
+      <c r="BR6">
+        <v>0</v>
+      </c>
+      <c r="BS6">
+        <v>0</v>
+      </c>
+      <c r="BT6">
+        <v>0</v>
+      </c>
+      <c r="BU6">
+        <v>0</v>
+      </c>
+      <c r="BV6">
+        <v>0</v>
+      </c>
+      <c r="BW6">
+        <v>0</v>
+      </c>
+      <c r="BX6">
+        <v>0</v>
+      </c>
+      <c r="BY6">
+        <v>0</v>
+      </c>
+      <c r="BZ6">
+        <v>0</v>
+      </c>
+      <c r="CA6">
+        <v>0</v>
+      </c>
+      <c r="CB6">
+        <v>0</v>
+      </c>
+      <c r="CC6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1215,8 +2082,152 @@
       <c r="AG7">
         <v>0</v>
       </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>0</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="AZ7">
+        <v>0</v>
+      </c>
+      <c r="BA7">
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <v>0</v>
+      </c>
+      <c r="BC7">
+        <v>0</v>
+      </c>
+      <c r="BD7">
+        <v>0</v>
+      </c>
+      <c r="BE7">
+        <v>0</v>
+      </c>
+      <c r="BF7">
+        <v>0</v>
+      </c>
+      <c r="BG7">
+        <v>0</v>
+      </c>
+      <c r="BH7">
+        <v>0</v>
+      </c>
+      <c r="BI7">
+        <v>0</v>
+      </c>
+      <c r="BJ7">
+        <v>0</v>
+      </c>
+      <c r="BK7">
+        <v>0</v>
+      </c>
+      <c r="BL7">
+        <v>0</v>
+      </c>
+      <c r="BM7">
+        <v>0</v>
+      </c>
+      <c r="BN7">
+        <v>0</v>
+      </c>
+      <c r="BO7">
+        <v>0</v>
+      </c>
+      <c r="BP7">
+        <v>0</v>
+      </c>
+      <c r="BQ7">
+        <v>0</v>
+      </c>
+      <c r="BR7">
+        <v>0</v>
+      </c>
+      <c r="BS7">
+        <v>0</v>
+      </c>
+      <c r="BT7">
+        <v>0</v>
+      </c>
+      <c r="BU7">
+        <v>0</v>
+      </c>
+      <c r="BV7">
+        <v>0</v>
+      </c>
+      <c r="BW7">
+        <v>0</v>
+      </c>
+      <c r="BX7">
+        <v>0</v>
+      </c>
+      <c r="BY7">
+        <v>0</v>
+      </c>
+      <c r="BZ7">
+        <v>0</v>
+      </c>
+      <c r="CA7">
+        <v>0</v>
+      </c>
+      <c r="CB7">
+        <v>0</v>
+      </c>
+      <c r="CC7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1316,8 +2327,152 @@
       <c r="AG8" s="3">
         <v>0</v>
       </c>
+      <c r="AH8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BI8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BM8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BO8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BP8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BQ8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BR8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BS8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BT8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BU8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BV8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BX8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BY8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BZ8" s="3">
+        <v>0</v>
+      </c>
+      <c r="CA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="CB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="CC8" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:81" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1415,6 +2570,150 @@
         <v>0</v>
       </c>
       <c r="AG9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BF9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BH9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BI9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BK9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BM9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BO9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BP9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BQ9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BR9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BS9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BT9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BU9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BV9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BX9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BY9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BZ9" s="3">
+        <v>0</v>
+      </c>
+      <c r="CA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="CB9" s="3">
+        <v>0</v>
+      </c>
+      <c r="CC9" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>